<commit_message>
projeto de execução e relatório prontos
</commit_message>
<xml_diff>
--- a/Projeto de teste.xlsx
+++ b/Projeto de teste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmachado/Downloads/Teste e configuração de software/-GLJ-Projeto-de-teste-casa-de-leila-o/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenk\Documents\-GLJ-Projeto-de-teste-casa-de-leila-o\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AF38AF-0A38-1649-9F27-D30B541B4D0E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7AD7F1-A3A5-4474-ABA7-E818BB3220B3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15860" activeTab="7" xr2:uid="{7F1A206E-AA9C-E14E-852A-6C40D7A73973}"/>
+    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="15855" firstSheet="1" activeTab="1" xr2:uid="{7F1A206E-AA9C-E14E-852A-6C40D7A73973}"/>
   </bookViews>
   <sheets>
     <sheet name="UC001" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,23 @@
     <sheet name="UC004" sheetId="4" r:id="rId7"/>
     <sheet name="UC004-dados" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="82">
   <si>
     <t>TC ID</t>
   </si>
@@ -202,9 +208,6 @@
     <t>WM2vrd6M77wTL</t>
   </si>
   <si>
-    <t>joanantha gabriel luan</t>
-  </si>
-  <si>
     <t>Seu Nome</t>
   </si>
   <si>
@@ -275,6 +278,12 @@
   </si>
   <si>
     <t>gljfnr@gmail.com</t>
+  </si>
+  <si>
+    <t>gljfnrgmail.com</t>
+  </si>
+  <si>
+    <t>566430c214@mailox.fun</t>
   </si>
 </sst>
 </file>
@@ -376,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -421,9 +430,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -440,7 +450,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -738,19 +748,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB330AC0-ADFC-D64E-9E57-D9D7883F2CD1}">
   <dimension ref="A1:XFD5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16384" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -809,7 +819,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -868,7 +878,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16384" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -927,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16384" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -986,7 +996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
@@ -17362,27 +17372,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96048EB0-8AC3-DF45-9E61-0C8D05E1CFB6}">
   <dimension ref="A1:XFD5"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.125" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.625" customWidth="1"/>
+    <col min="9" max="9" width="18.125" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="30.33203125" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.125" customWidth="1"/>
+    <col min="14" max="14" width="30.375" customWidth="1"/>
+    <col min="15" max="15" width="19.375" customWidth="1"/>
+    <col min="17" max="17" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16384" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -17441,7 +17451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -17452,7 +17462,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>41</v>
@@ -17466,11 +17476,11 @@
       <c r="H2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>46</v>
+      <c r="I2" s="4">
+        <v>12214963448</v>
+      </c>
+      <c r="J2" s="4">
+        <v>404710499</v>
       </c>
       <c r="K2" s="13">
         <v>34657</v>
@@ -17500,7 +17510,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16384" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -17510,8 +17520,8 @@
       <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>80</v>
+      <c r="D3" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>41</v>
@@ -17523,11 +17533,11 @@
       <c r="H3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>46</v>
+      <c r="I3" s="4">
+        <v>12214963448</v>
+      </c>
+      <c r="J3" s="4">
+        <v>404710499</v>
       </c>
       <c r="K3" s="13">
         <v>34657</v>
@@ -17557,7 +17567,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16384" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -17568,7 +17578,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>41</v>
@@ -17582,11 +17592,11 @@
       <c r="H4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>46</v>
+      <c r="I4" s="4">
+        <v>12214963448</v>
+      </c>
+      <c r="J4" s="4">
+        <v>404710499</v>
       </c>
       <c r="K4" s="13">
         <v>34657</v>
@@ -17616,7 +17626,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
@@ -33986,8 +33996,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{E9B5282E-0A2A-7C41-B7B1-3CCC88D6855A}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{3785D19E-CD1F-474C-ADFB-BD23EFBDEBD1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -33996,15 +34008,15 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -34021,7 +34033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -34038,9 +34050,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>35</v>
@@ -34055,9 +34067,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
@@ -34072,9 +34084,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>36</v>
@@ -34098,18 +34110,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7215E3-267C-DC4B-BF5D-016568581749}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="242" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -34126,7 +34138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -34137,13 +34149,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -34160,7 +34172,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -34177,7 +34189,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -34188,7 +34200,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>55</v>
@@ -34197,6 +34209,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{B33D6E50-454D-CF42-8E39-A7EACFED3998}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{FA16EB92-B092-4E42-A237-5EA5A1DF3533}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34207,16 +34220,16 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -34275,9 +34288,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>37</v>
@@ -34334,9 +34347,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>38</v>
@@ -34393,9 +34406,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>39</v>
@@ -34452,7 +34465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="9"/>
@@ -34467,27 +34480,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F162A84-30D4-4C4F-90DA-7748B8F348C6}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="B1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.625" customWidth="1"/>
+    <col min="4" max="4" width="22.125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="8" width="27.33203125" customWidth="1"/>
-    <col min="9" max="10" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
+    <col min="7" max="8" width="27.375" customWidth="1"/>
+    <col min="9" max="10" width="21.875" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.375" customWidth="1"/>
     <col min="14" max="14" width="37.5" customWidth="1"/>
-    <col min="15" max="15" width="24.33203125" customWidth="1"/>
-    <col min="16" max="16" width="28.1640625" customWidth="1"/>
-    <col min="17" max="17" width="21.33203125" customWidth="1"/>
+    <col min="15" max="15" width="24.375" customWidth="1"/>
+    <col min="16" max="16" width="28.125" customWidth="1"/>
+    <col min="17" max="17" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -34546,7 +34559,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -34557,7 +34570,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>41</v>
@@ -34569,7 +34582,7 @@
         <v>43</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>45</v>
@@ -34605,7 +34618,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -34616,7 +34629,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>41</v>
@@ -34630,7 +34643,9 @@
       <c r="H3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="J3" s="4" t="s">
         <v>46</v>
       </c>
@@ -34640,9 +34655,7 @@
       <c r="L3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="4">
-        <v>54530340</v>
-      </c>
+      <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
         <v>48</v>
       </c>
@@ -34662,7 +34675,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -34673,7 +34686,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>41</v>
@@ -34734,12 +34747,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -34750,33 +34763,33 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>64</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>40</v>
@@ -34809,9 +34822,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>38</v>
@@ -34853,20 +34866,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F55000-E026-744A-920E-0DD423779AF1}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="E1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.375" customWidth="1"/>
     <col min="11" max="11" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -34877,33 +34890,33 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>64</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>40</v>
@@ -34912,33 +34925,33 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>79</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>38</v>
@@ -34948,28 +34961,32 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{8F6A8EF5-BB5E-40DD-978A-E829EC89D45E}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{5BE45CAE-6000-4148-B82D-3CE9DF31D801}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correção dos documentos de execução, caso de teste e relatório
</commit_message>
<xml_diff>
--- a/Projeto de teste.xlsx
+++ b/Projeto de teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenk\Documents\-GLJ-Projeto-de-teste-casa-de-leila-o\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7AD7F1-A3A5-4474-ABA7-E818BB3220B3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E85F9A-07AA-4BA3-9186-A1D9438D83F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="15855" firstSheet="1" activeTab="1" xr2:uid="{7F1A206E-AA9C-E14E-852A-6C40D7A73973}"/>
+    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="15855" firstSheet="1" activeTab="7" xr2:uid="{7F1A206E-AA9C-E14E-852A-6C40D7A73973}"/>
   </bookViews>
   <sheets>
     <sheet name="UC001" sheetId="1" r:id="rId1"/>
@@ -17372,8 +17372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96048EB0-8AC3-DF45-9E61-0C8D05E1CFB6}">
   <dimension ref="A1:XFD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -34111,7 +34111,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -34866,8 +34866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F55000-E026-744A-920E-0DD423779AF1}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>